<commit_message>
Implemented sprites and fonts. still wip
</commit_message>
<xml_diff>
--- a/Documents/Aanwezigheid Game labs 2 Orphanage.xlsx
+++ b/Documents/Aanwezigheid Game labs 2 Orphanage.xlsx
@@ -632,7 +632,7 @@
       </c>
       <c r="B1" s="5">
         <f>SUM('Week 20:Week 27'!B8)</f>
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -679,7 +679,7 @@
       </c>
       <c r="B4" s="5">
         <f>SUM('Week 20:Week 27'!C8, F4)</f>
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C4" s="19">
         <f>B4/(B1/100)</f>
@@ -709,11 +709,11 @@
       </c>
       <c r="B5" s="5">
         <f>SUM('Week 20:Week 27'!D8,F5)</f>
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C5" s="19">
         <f>B5/(B1/100)</f>
-        <v>66.666666666666671</v>
+        <v>80.952380952380949</v>
       </c>
       <c r="D5" s="5">
         <f>SUM('Week 20:Week 27'!D11)</f>
@@ -721,7 +721,7 @@
       </c>
       <c r="E5" s="19">
         <f>D5/(B1/100)</f>
-        <v>33.333333333333336</v>
+        <v>19.047619047619047</v>
       </c>
       <c r="F5" s="14">
         <f>SUM('Week 20:Week 27'!D12)</f>
@@ -739,7 +739,7 @@
       </c>
       <c r="B6" s="5">
         <f>SUM('Week 20:Week 27'!E8,F6)</f>
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C6" s="19">
         <f>B6/(B1/100)</f>
@@ -1213,7 +1213,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1260,10 +1260,18 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="B3" s="5">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5">
+        <v>4</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="H3" s="1"/>
     </row>
@@ -1271,10 +1279,18 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="H4" s="1"/>
     </row>
@@ -1282,10 +1298,18 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="H5" s="1"/>
     </row>
@@ -1293,10 +1317,18 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="B6" s="5">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <v>8</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="H6" s="1"/>
     </row>
@@ -1316,19 +1348,19 @@
       </c>
       <c r="B8" s="5">
         <f>SUM(B2:B6)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" ref="C8:E8" si="0">SUM(C2:C6)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="8"/>
@@ -1394,7 +1426,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Alot of Slab problems.
Changed Slab from world to camera space to resolve all problems. Slab in hand idea will be scrapped.
</commit_message>
<xml_diff>
--- a/Documents/Aanwezigheid Game labs 2 Orphanage.xlsx
+++ b/Documents/Aanwezigheid Game labs 2 Orphanage.xlsx
@@ -709,19 +709,19 @@
       </c>
       <c r="B5" s="5">
         <f>SUM('Week 20:Week 27'!D8,F5)</f>
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="19">
         <f>B5/(B1/100)</f>
-        <v>86.666666666666671</v>
+        <v>83.333333333333343</v>
       </c>
       <c r="D5" s="5">
         <f>SUM('Week 20:Week 27'!D11)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E5" s="19">
         <f>D5/(B1/100)</f>
-        <v>13.333333333333334</v>
+        <v>16.666666666666668</v>
       </c>
       <c r="F5" s="14">
         <f>SUM('Week 20:Week 27'!D12)</f>
@@ -1429,7 +1429,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1500,7 +1500,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" s="5">
         <v>2</v>
@@ -1565,12 +1565,12 @@
         <v>18</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" ref="C8:E8" si="0">SUM(C2:C6)</f>
+        <f t="shared" ref="C8:D8" si="0">SUM(C2:C6)</f>
         <v>18</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="5">
         <v>4</v>
@@ -1606,6 +1606,9 @@
         <v>11</v>
       </c>
       <c r="B11" s="7"/>
+      <c r="D11">
+        <v>2</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>

</xml_diff>

<commit_message>
Added npc's and started work on dialogue
</commit_message>
<xml_diff>
--- a/Documents/Aanwezigheid Game labs 2 Orphanage.xlsx
+++ b/Documents/Aanwezigheid Game labs 2 Orphanage.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sepi\Desktop\Orphanage\Documents\"/>
@@ -679,11 +679,11 @@
       </c>
       <c r="B4" s="5">
         <f>SUM('Week 20:Week 27'!C8, F4)</f>
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C4" s="19">
         <f>B4/(B1/100)</f>
-        <v>97.435897435897431</v>
+        <v>120.51282051282051</v>
       </c>
       <c r="D4" s="5">
         <f>SUM('Week 20:Week 27'!C11)</f>
@@ -709,11 +709,11 @@
       </c>
       <c r="B5" s="5">
         <f>SUM('Week 20:Week 27'!D8,F5)</f>
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C5" s="19">
         <f>B5/(B1/100)</f>
-        <v>82.051282051282044</v>
+        <v>105.12820512820512</v>
       </c>
       <c r="D5" s="5">
         <f>SUM('Week 20:Week 27'!D11)</f>
@@ -739,11 +739,11 @@
       </c>
       <c r="B6" s="5">
         <f>SUM('Week 20:Week 27'!E8,F6)</f>
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="C6" s="19">
         <f>B6/(B1/100)</f>
-        <v>100</v>
+        <v>123.07692307692307</v>
       </c>
       <c r="D6" s="5">
         <f>SUM('Week 20:Week 27'!E11)</f>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1909,9 +1909,15 @@
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5">
+        <v>4</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="H3" s="1"/>
     </row>
@@ -1920,9 +1926,15 @@
         <v>2</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="H4" s="1"/>
     </row>
@@ -1931,9 +1943,15 @@
         <v>3</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="H5" s="1"/>
     </row>
@@ -1942,9 +1960,15 @@
         <v>4</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="C6" s="5">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <v>8</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="H6" s="1"/>
     </row>
@@ -1968,15 +1992,15 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" ref="C8:E8" si="0">SUM(C2:C6)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="8"/>

</xml_diff>